<commit_message>
Adding new field to schema definitions: multivalue, separator. Incrementing schema version.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.3.xlsx
+++ b/schema_definitions/template_schema_v1.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EC7B55-F8DC-0A4A-BBDA-E3D9D2EF1D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B098F733-B0F5-CE4A-94E4-C22E12D07358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38600" yWindow="2280" windowWidth="38240" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="28800" yWindow="2280" windowWidth="48040" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -496,9 +496,6 @@
     <t>cohort_id</t>
   </si>
   <si>
-    <t>Comma separated list of cohort specific identifier(s) issued to this research study</t>
-  </si>
-  <si>
     <t>UK Biobank ID</t>
   </si>
   <si>
@@ -517,9 +514,6 @@
     <t>Cohort(s)</t>
   </si>
   <si>
-    <t>Comma separated list of cohort(s) represented in the discovery sample</t>
-  </si>
-  <si>
     <t>Genome assembly for the summary statistics</t>
   </si>
   <si>
@@ -578,6 +572,12 @@
   </si>
   <si>
     <t>|</t>
+  </si>
+  <si>
+    <t>Cohort(s) represented in the discovery sample</t>
+  </si>
+  <si>
+    <t>Cohort specific identifier(s) issued to this research study</t>
   </si>
 </sst>
 </file>
@@ -990,14 +990,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.83203125" style="5" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="5" bestFit="1" customWidth="1"/>
@@ -1025,10 +1025,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
@@ -1049,10 +1049,10 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>9</v>
@@ -1110,7 +1110,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>143</v>
@@ -1152,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>26</v>
@@ -1190,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
         <v>44</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>35</v>
@@ -1374,7 +1374,7 @@
         <v>54</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M11" s="7" t="b">
         <v>0</v>
@@ -1441,7 +1441,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1516,7 +1516,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>1</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>62</v>
@@ -1571,10 +1571,10 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -1592,7 +1592,7 @@
         <v>24</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M18" s="10" t="b">
         <v>0</v>
@@ -1603,7 +1603,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -1630,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -1638,7 +1638,7 @@
         <v>149</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -1659,13 +1659,13 @@
         <v>150</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M20" s="7" t="b">
         <v>1</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -1673,7 +1673,7 @@
         <v>151</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -1691,16 +1691,16 @@
         <v>24</v>
       </c>
       <c r="I21" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="L21" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>154</v>
-      </c>
       <c r="M21" s="7" t="b">
         <v>1</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1750,10 +1750,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
@@ -1774,10 +1774,10 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>9</v>
@@ -1929,7 +1929,7 @@
         <v>24</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M6" s="10" t="b">
         <v>0</v>
@@ -1988,7 +1988,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>125</v>
@@ -2020,7 +2020,7 @@
         <v>24</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>122</v>
@@ -2282,10 +2282,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>3</v>
@@ -2306,10 +2306,10 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>9</v>
@@ -2349,7 +2349,7 @@
         <v>100</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C3" s="7" t="b">
         <v>1</v>
@@ -2367,7 +2367,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>99</v>
@@ -2532,10 +2532,10 @@
         <v>1</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2590,7 +2590,7 @@
         <v>24</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M10" s="7" t="b">
         <v>0</v>
@@ -2628,7 +2628,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3665,10 +3665,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
@@ -3689,10 +3689,10 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>9</v>
@@ -3775,7 +3775,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>68</v>
@@ -3807,7 +3807,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>65</v>

</xml_diff>